<commit_message>
Weitere Umbauten an der Datenbank. Tests würden derzeit nicht laufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Neuanlage Arbeitslosenversicherungsbeitraege.xlsx
+++ b/src/main/Mitarbeiterdaten/Neuanlage Arbeitslosenversicherungsbeitraege.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE07D6D-4EEC-472D-A9D4-3D8C0ED64340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315BE76E-6D57-48DB-BBA8-2B5800CA93E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>Beitragsbemessungsgrenze AV West</t>
   </si>
   <si>
-    <t>Mitarbeitertyp</t>
-  </si>
-  <si>
-    <t>Angestellter</t>
+    <t>Eintragungsdatum</t>
+  </si>
+  <si>
+    <t>15.12.2023</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>